<commit_message>
Fix convert uploaded data type to google charts format. closed #9.
</commit_message>
<xml_diff>
--- a/excelPath/test/datatable.xlsx
+++ b/excelPath/test/datatable.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>name(string)</t>
   </si>
@@ -46,64 +46,61 @@
     <t>Eng</t>
   </si>
   <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>2005-03-19</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>2007-12-02 15:56:00</t>
+  </si>
+  <si>
     <t>Dave</t>
   </si>
   <si>
+    <t>13:01:30.123</t>
+  </si>
+  <si>
+    <t>500.5</t>
+  </si>
+  <si>
+    <t>2006-04-19</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>2005-03-09 12:30:00.32</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>09:30:05</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>2005-10-10</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>null</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Dana</t>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>12:00:00</t>
-  </si>
-  <si>
-    <t>2005-03-19</t>
-  </si>
-  <si>
-    <t>2006-04-19</t>
-  </si>
-  <si>
-    <t>2005-10-10</t>
-  </si>
-  <si>
-    <t>2002-10-10</t>
-  </si>
-  <si>
-    <t>2004-09-08</t>
-  </si>
-  <si>
-    <t>2005-01-10</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>2007-12-02 15:56:00</t>
-  </si>
-  <si>
-    <t>2005-03-09 12:30:00</t>
-  </si>
-  <si>
-    <t>2007-12-30 14:40:00</t>
   </si>
 </sst>
 </file>
@@ -112,11 +109,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,21 +136,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -202,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,20 +297,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -439,211 +428,176 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <sheetPr>
+    <tabColor rgb="FFC0000"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1">
-        <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1">
-        <v>500</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1">
-        <v>600</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1">
-        <v>30</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1">
-        <v>400</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="H4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1">
-        <v>350</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1">
-        <v>800</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>